<commit_message>
Important final touches and sent the file to client
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/1_Data/Schedule.xlsx
+++ b/6_Inventory_Management/1_Data/Schedule.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>Many features added for reporting - Rev03 sent</t>
+  </si>
+  <si>
+    <t>Updates based on comments</t>
+  </si>
+  <si>
+    <t>04 - 12 - 2019</t>
+  </si>
+  <si>
+    <t>Lot of feature updates and reports update</t>
+  </si>
+  <si>
+    <t>07 - 12 - 2019</t>
   </si>
 </sst>
 </file>
@@ -604,20 +616,20 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="5" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -945,10 +957,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J31"/>
+  <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -968,22 +980,22 @@
   <sheetData>
     <row r="1" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:10" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1031,7 +1043,7 @@
       <c r="E7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="30">
         <v>3</v>
       </c>
       <c r="G7" s="12"/>
@@ -1052,7 +1064,7 @@
       <c r="E8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="30">
         <v>3</v>
       </c>
       <c r="G8" s="12"/>
@@ -1073,7 +1085,7 @@
       <c r="E9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="30">
         <v>3</v>
       </c>
       <c r="G9" s="12"/>
@@ -1094,7 +1106,7 @@
       <c r="E10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="30">
         <v>1</v>
       </c>
       <c r="G10" s="12"/>
@@ -1115,7 +1127,7 @@
       <c r="E11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="30">
         <v>1</v>
       </c>
       <c r="G11" s="12"/>
@@ -1136,7 +1148,7 @@
       <c r="E12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="30">
         <v>1.5</v>
       </c>
       <c r="G12" s="12"/>
@@ -1157,7 +1169,7 @@
       <c r="E13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="30">
         <v>2</v>
       </c>
       <c r="G13" s="12"/>
@@ -1178,7 +1190,7 @@
       <c r="E14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="30">
         <v>3</v>
       </c>
       <c r="G14" s="12"/>
@@ -1199,7 +1211,7 @@
       <c r="E15" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="30">
         <v>4</v>
       </c>
       <c r="G15" s="12"/>
@@ -1220,7 +1232,7 @@
       <c r="E16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="30">
         <v>5</v>
       </c>
       <c r="G16" s="12"/>
@@ -1241,7 +1253,7 @@
       <c r="E17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="30">
         <v>1.5</v>
       </c>
       <c r="G17" s="12"/>
@@ -1262,7 +1274,7 @@
       <c r="E18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="30">
         <v>5</v>
       </c>
       <c r="G18" s="12"/>
@@ -1271,38 +1283,80 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="33"/>
+      <c r="B19" s="14">
+        <v>13</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="30">
+        <v>2</v>
+      </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="34"/>
+    <row r="20" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="14">
+        <v>14</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="30">
+        <v>5</v>
+      </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="23" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="31" spans="2:10" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="4"/>
-      <c r="C31" s="1"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+    <row r="21" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="25" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+    </row>
+    <row r="33" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" s="1"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Need to send this iteration to client for actual input or usage of data
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/1_Data/Schedule.xlsx
+++ b/6_Inventory_Management/1_Data/Schedule.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>07 - 12 - 2019</t>
+  </si>
+  <si>
+    <t>Preparation for actual data input</t>
+  </si>
+  <si>
+    <t>08 - 12 - 2019</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -577,9 +583,6 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -618,9 +621,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -959,8 +959,8 @@
   </sheetPr>
   <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -980,22 +980,22 @@
   <sheetData>
     <row r="1" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:10" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1008,7 +1008,7 @@
       <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -1020,11 +1020,11 @@
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="3"/>
@@ -1037,13 +1037,13 @@
       <c r="C7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="30">
+      <c r="E7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="29">
         <v>3</v>
       </c>
       <c r="G7" s="12"/>
@@ -1058,13 +1058,13 @@
       <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="30">
+      <c r="E8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="29">
         <v>3</v>
       </c>
       <c r="G8" s="12"/>
@@ -1079,13 +1079,13 @@
       <c r="C9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="30">
+      <c r="E9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="29">
         <v>3</v>
       </c>
       <c r="G9" s="12"/>
@@ -1100,13 +1100,13 @@
       <c r="C10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="30">
+      <c r="E10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="29">
         <v>1</v>
       </c>
       <c r="G10" s="12"/>
@@ -1121,13 +1121,13 @@
       <c r="C11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="30">
+      <c r="E11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="29">
         <v>1</v>
       </c>
       <c r="G11" s="12"/>
@@ -1142,13 +1142,13 @@
       <c r="C12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="30">
+      <c r="E12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="29">
         <v>1.5</v>
       </c>
       <c r="G12" s="12"/>
@@ -1163,13 +1163,13 @@
       <c r="C13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="30">
+      <c r="E13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="29">
         <v>2</v>
       </c>
       <c r="G13" s="12"/>
@@ -1184,13 +1184,13 @@
       <c r="C14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="30">
+      <c r="E14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="29">
         <v>3</v>
       </c>
       <c r="G14" s="12"/>
@@ -1205,13 +1205,13 @@
       <c r="C15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="30">
+      <c r="E15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="29">
         <v>4</v>
       </c>
       <c r="G15" s="12"/>
@@ -1226,13 +1226,13 @@
       <c r="C16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="30">
+      <c r="E16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="29">
         <v>5</v>
       </c>
       <c r="G16" s="12"/>
@@ -1247,13 +1247,13 @@
       <c r="C17" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="30">
+      <c r="E17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="29">
         <v>1.5</v>
       </c>
       <c r="G17" s="12"/>
@@ -1268,13 +1268,13 @@
       <c r="C18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="30">
+      <c r="E18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="29">
         <v>5</v>
       </c>
       <c r="G18" s="12"/>
@@ -1289,13 +1289,13 @@
       <c r="C19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="30">
+      <c r="E19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="29">
         <v>2</v>
       </c>
       <c r="G19" s="12"/>
@@ -1310,13 +1310,13 @@
       <c r="C20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="30">
+      <c r="E20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="29">
         <v>5</v>
       </c>
       <c r="G20" s="12"/>
@@ -1325,22 +1325,32 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="31"/>
+      <c r="B21" s="14">
+        <v>15</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="29">
+        <v>4</v>
+      </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="32"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="3"/>

</xml_diff>

<commit_message>
Important critical updates - Working live with client
Signed-off-by: syedmeesamali <syedmeesamali@yahoo.com>
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/1_Data/Schedule.xlsx
+++ b/6_Inventory_Management/1_Data/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\VBA_Programming\6_Inventory_Management\1_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B316C910-D39E-4D98-8E39-14B15A9E4510}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDAD6AA-1F6B-4C1D-9628-E33F35542768}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -71,9 +71,6 @@
     <t>16 - 11 - 2019</t>
   </si>
   <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
     <t>Linking and testing</t>
   </si>
   <si>
@@ -156,6 +153,18 @@
   </si>
   <si>
     <t>30 - 12 - 2019</t>
+  </si>
+  <si>
+    <t>Revision-06 - Bug fixes</t>
+  </si>
+  <si>
+    <t>31 - 12 - 2019</t>
+  </si>
+  <si>
+    <t>Revision-07 - Previous file check &amp; bug fixes</t>
+  </si>
+  <si>
+    <t>02 - 01 - 2020</t>
   </si>
 </sst>
 </file>
@@ -587,9 +596,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -635,13 +641,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1004,10 +1013,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J35"/>
+  <dimension ref="B1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1055,7 +1064,7 @@
       <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -1066,32 +1075,32 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23"/>
+    <row r="6" spans="2:10" s="13" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="14">
+      <c r="B7" s="32">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="29">
-        <v>3</v>
+      <c r="E7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="28">
+        <v>2</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1099,20 +1108,20 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="14">
+      <c r="B8" s="32">
         <v>2</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="29">
-        <v>3</v>
+      <c r="E8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="28">
+        <v>2</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -1120,20 +1129,20 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="14">
+      <c r="B9" s="32">
         <v>3</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="29">
-        <v>3</v>
+      <c r="E9" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="28">
+        <v>2</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -1141,19 +1150,19 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="14">
+      <c r="B10" s="32">
         <v>4</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="29">
+      <c r="C10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="28">
         <v>1</v>
       </c>
       <c r="G10" s="12"/>
@@ -1162,19 +1171,19 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="14">
+      <c r="B11" s="32">
         <v>5</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="29">
+      <c r="C11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="28">
         <v>1</v>
       </c>
       <c r="G11" s="12"/>
@@ -1183,19 +1192,19 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="14">
+      <c r="B12" s="32">
         <v>6</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="29">
+      <c r="C12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="28">
         <v>1.5</v>
       </c>
       <c r="G12" s="12"/>
@@ -1204,20 +1213,20 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="14">
+      <c r="B13" s="32">
         <v>7</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="29">
-        <v>2</v>
+      <c r="E13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="28">
+        <v>1.5</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -1225,20 +1234,20 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="14">
+      <c r="B14" s="32">
         <v>8</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="29">
-        <v>3</v>
+      <c r="C14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="28">
+        <v>2</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -1246,20 +1255,20 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="14">
-        <v>9</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="28" t="s">
+      <c r="B15" s="32">
+        <v>9</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="29">
-        <v>4</v>
+      <c r="D15" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="28">
+        <v>3</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
@@ -1267,20 +1276,20 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="14">
+      <c r="B16" s="32">
         <v>10</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="29">
-        <v>5</v>
+      <c r="D16" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="28">
+        <v>3</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -1288,19 +1297,19 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="14">
+      <c r="B17" s="32">
         <v>11</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="29">
+      <c r="E17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="28">
         <v>1.5</v>
       </c>
       <c r="G17" s="12"/>
@@ -1309,20 +1318,20 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="14">
+      <c r="B18" s="32">
         <v>12</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="28" t="s">
+      <c r="C18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="29">
-        <v>5</v>
+      <c r="D18" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="28">
+        <v>4</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
@@ -1330,19 +1339,19 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="14">
+      <c r="B19" s="32">
         <v>13</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="29">
+      <c r="E19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="28">
         <v>2</v>
       </c>
       <c r="G19" s="12"/>
@@ -1351,19 +1360,19 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="14">
+      <c r="B20" s="32">
         <v>14</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="29">
+      <c r="E20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="28">
         <v>5</v>
       </c>
       <c r="G20" s="12"/>
@@ -1372,20 +1381,20 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="14">
+      <c r="B21" s="32">
         <v>15</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="29">
-        <v>4</v>
+      <c r="E21" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="28">
+        <v>3</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -1393,19 +1402,19 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="14">
+      <c r="B22" s="32">
         <v>16</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="29">
+      <c r="E22" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="28">
         <v>2</v>
       </c>
       <c r="G22" s="12"/>
@@ -1414,19 +1423,19 @@
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="14">
+      <c r="B23" s="32">
         <v>17</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="29">
+      <c r="E23" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="28">
         <v>3</v>
       </c>
       <c r="G23" s="12"/>
@@ -1434,31 +1443,73 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="32">
-        <f>SUM(F7:F23)</f>
-        <v>49</v>
+    <row r="24" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="32">
+        <v>18</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="28">
+        <v>1</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="27" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="35" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="4"/>
-      <c r="C35" s="1"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
+    <row r="25" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="32">
+        <v>19</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="28">
+        <v>1</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="29">
+        <f>SUM(F7:F25)</f>
+        <v>41.5</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="29" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="37" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="C37" s="1"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Schedule update - MoU received finally - Rev09 submitted
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/1_Data/Schedule.xlsx
+++ b/6_Inventory_Management/1_Data/Schedule.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\VBA_Programming\6_Inventory_Management\1_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\VBA_Programming\6_Inventory_Management\1_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDAD6AA-1F6B-4C1D-9628-E33F35542768}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="IMS_System" sheetId="12" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <definedName name="_Fill" hidden="1">#REF!</definedName>
     <definedName name="wrn.OCS._.REPORT." hidden="1">{#N/A,#N/A,FALSE,"Cover";#N/A,#N/A,FALSE,"Index";#N/A,#N/A,FALSE,"Spec";#N/A,#N/A,FALSE,"Breakdown";#N/A,#N/A,FALSE,"Cost Plan"}</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -165,12 +164,24 @@
   </si>
   <si>
     <t>02 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>Revision-08 - Re-import related issues</t>
+  </si>
+  <si>
+    <t>05 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>Revision-09 _ Over-ride function added</t>
+  </si>
+  <si>
+    <t>07 - 01 - 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -644,31 +655,31 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comma" xfId="12" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Comma 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Comma 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Comma 3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Comma 4" xfId="11" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma 2" xfId="2"/>
+    <cellStyle name="Comma 2 2" xfId="6"/>
+    <cellStyle name="Comma 3" xfId="4"/>
+    <cellStyle name="Comma 3 2" xfId="8"/>
+    <cellStyle name="Comma 4" xfId="11"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 3 2" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 4" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Percent 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 3 2" xfId="7"/>
+    <cellStyle name="Normal 4" xfId="10"/>
+    <cellStyle name="Normal 5" xfId="13"/>
+    <cellStyle name="Percent 2" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -765,23 +776,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -817,23 +811,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1009,14 +986,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J37"/>
+  <dimension ref="B1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1036,22 +1013,22 @@
   <sheetData>
     <row r="1" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:10" s="11" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1087,7 +1064,7 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="32">
+      <c r="B7" s="30">
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -1108,7 +1085,7 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="32">
+      <c r="B8" s="30">
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1129,7 +1106,7 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="32">
+      <c r="B9" s="30">
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -1150,7 +1127,7 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="32">
+      <c r="B10" s="30">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1171,7 +1148,7 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="32">
+      <c r="B11" s="30">
         <v>5</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -1192,7 +1169,7 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="32">
+      <c r="B12" s="30">
         <v>6</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1213,7 +1190,7 @@
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="32">
+      <c r="B13" s="30">
         <v>7</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -1234,7 +1211,7 @@
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="32">
+      <c r="B14" s="30">
         <v>8</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -1255,7 +1232,7 @@
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="32">
+      <c r="B15" s="30">
         <v>9</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -1276,7 +1253,7 @@
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="32">
+      <c r="B16" s="30">
         <v>10</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -1297,7 +1274,7 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="32">
+      <c r="B17" s="30">
         <v>11</v>
       </c>
       <c r="C17" s="14" t="s">
@@ -1318,7 +1295,7 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="32">
+      <c r="B18" s="30">
         <v>12</v>
       </c>
       <c r="C18" s="14" t="s">
@@ -1339,7 +1316,7 @@
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="32">
+      <c r="B19" s="30">
         <v>13</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -1360,7 +1337,7 @@
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="32">
+      <c r="B20" s="30">
         <v>14</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -1381,7 +1358,7 @@
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="32">
+      <c r="B21" s="30">
         <v>15</v>
       </c>
       <c r="C21" s="14" t="s">
@@ -1402,7 +1379,7 @@
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="32">
+      <c r="B22" s="30">
         <v>16</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -1423,7 +1400,7 @@
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="32">
+      <c r="B23" s="30">
         <v>17</v>
       </c>
       <c r="C23" s="14" t="s">
@@ -1444,7 +1421,7 @@
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="32">
+      <c r="B24" s="30">
         <v>18</v>
       </c>
       <c r="C24" s="14" t="s">
@@ -1465,7 +1442,7 @@
       <c r="J24" s="3"/>
     </row>
     <row r="25" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="32">
+      <c r="B25" s="30">
         <v>19</v>
       </c>
       <c r="C25" s="14" t="s">
@@ -1485,31 +1462,73 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="29">
-        <f>SUM(F7:F25)</f>
-        <v>41.5</v>
+    <row r="26" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="30">
+        <v>20</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="28">
+        <v>1</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="29" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="37" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="4"/>
-      <c r="C37" s="1"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
+    <row r="27" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="30">
+        <v>21</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="28">
+        <v>1.5</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="29">
+        <f>SUM(F7:F27)</f>
+        <v>44</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="31" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="39" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" s="1"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Important critical updates - need to RAISE INVOICE for 50%
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/1_Data/Schedule.xlsx
+++ b/6_Inventory_Management/1_Data/Schedule.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Description</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>07 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>Revision-10_File duplicate checks &amp; Date related</t>
+  </si>
+  <si>
+    <t>13 - 01 - 2020</t>
   </si>
 </sst>
 </file>
@@ -990,10 +996,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J39"/>
+  <dimension ref="B1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1504,31 +1510,52 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="29">
-        <f>SUM(F7:F27)</f>
-        <v>44</v>
+    <row r="28" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="30">
+        <v>22</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="28">
+        <v>2</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="31" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="39" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="4"/>
-      <c r="C39" s="1"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
+    <row r="29" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="29">
+        <f>SUM(F7:F28)</f>
+        <v>46</v>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="32" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="40" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" s="1"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Invoice sent to ali bhai - invoice # 001
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/1_Data/Schedule.xlsx
+++ b/6_Inventory_Management/1_Data/Schedule.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>Description</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>13 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>Revision-11_File duplicate checks updated</t>
+  </si>
+  <si>
+    <t>16 - 01 - 2020</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1002,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J40"/>
+  <dimension ref="B1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1531,31 +1537,52 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="29">
-        <f>SUM(F7:F28)</f>
-        <v>46</v>
+    <row r="29" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="30">
+        <v>23</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="28">
+        <v>1</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="32" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="40" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="4"/>
-      <c r="C40" s="1"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
+    <row r="30" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="29">
+        <f>SUM(F7:F29)</f>
+        <v>47</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="33" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+    </row>
+    <row r="41" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="1"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Some over-ride related updates
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/1_Data/Schedule.xlsx
+++ b/6_Inventory_Management/1_Data/Schedule.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -188,6 +188,48 @@
   </si>
   <si>
     <t>16 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>GUI App Overall design study</t>
+  </si>
+  <si>
+    <t>18 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>GUI App Reporting Design</t>
+  </si>
+  <si>
+    <t>20 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>GUI App SQL Server Database Design</t>
+  </si>
+  <si>
+    <t>25 - 01 - 2020</t>
+  </si>
+  <si>
+    <t>GUI App Layout and Basic Functions</t>
+  </si>
+  <si>
+    <t>04 - 02 - 2020</t>
+  </si>
+  <si>
+    <t>GUI App Reporting using ReportViewer</t>
+  </si>
+  <si>
+    <t>08 - 02 - 2020</t>
+  </si>
+  <si>
+    <t>GUI App Report + SQL Server Custom Reports</t>
+  </si>
+  <si>
+    <t>12 - 02 - 2020</t>
+  </si>
+  <si>
+    <t>GUI APP as IMS_Final : Final testing and Setup</t>
+  </si>
+  <si>
+    <t>15 - 02 - 2020</t>
   </si>
 </sst>
 </file>
@@ -197,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -300,6 +342,19 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -321,7 +376,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -559,6 +614,43 @@
       <bottom style="hair">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -578,7 +670,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -675,6 +767,27 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="17" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="18" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="5" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1002,10 +1115,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J41"/>
+  <dimension ref="B1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1558,31 +1671,212 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="29">
-        <f>SUM(F7:F29)</f>
-        <v>47</v>
+    <row r="30" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="30">
+        <v>24</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="28">
+        <v>2</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="33" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="41" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="4"/>
-      <c r="C41" s="1"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
+    <row r="31" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="30">
+        <v>25</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="28">
+        <v>2</v>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="30">
+        <v>26</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="28">
+        <v>1</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="30">
+        <v>27</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="28">
+        <v>1</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="30">
+        <v>28</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="28">
+        <v>1</v>
+      </c>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="30">
+        <v>29</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="28">
+        <v>2</v>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="30">
+        <v>30</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="28">
+        <v>2</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="30">
+        <v>31</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="28">
+        <v>3</v>
+      </c>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="30">
+        <v>32</v>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="2:10" s="13" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="29">
+        <f>SUM(F7:F38)</f>
+        <v>61</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="42" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+    </row>
+    <row r="50" spans="2:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="4"/>
+      <c r="C50" s="1"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>